<commit_message>
[Update] removing , in the xlsx files & csv files
[Update] removing , in the xlsx files & csv files
</commit_message>
<xml_diff>
--- a/Documents/Files/Item.xlsx
+++ b/Documents/Files/Item.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sparta_Coding_Club\TeamProject\TextRPG_TeamProject2nd\TextRPG_TeamProject2nd\Documents\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EEBC484-4903-4FAA-B05F-483A1A5722F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0F9F7E-271E-426D-B490-740EAA818A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28695" yWindow="16110" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,10 +109,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>커트시를 하는 듯 한, 우아한 움직임으로 사용하는 고양이 일족의 무기.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>캐트시 랜스</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -133,10 +129,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>토끼 농부들이 사용하는 낫. 낮에는 밭을 매고, 밤에는 수렵하는, 그들은 '노동자'다.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>1000|2003</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -380,6 +372,98 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>초보 모험가들이 자주 입는 복장. 초록색 옷에 초록색 모자가 특징이다. 전설 같은 건 없다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>모험가 복장</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>가격이 있어서 베테랑 모험가들이 자주 입는다. 푸른 상의가 특징이다. 자꾸 전설을 찾지 말아라.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>탐험가 복장</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>보랏빛 허리 망토가 특징인 장비. 세상을 구한 영웅의 옷을 모방했다는 전설이 있다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>구원자 복장</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>늑대 가죽</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>늑대들의 가죽을 그대로 뒤집어 쓴 것. 느낌을 살리기 위해서 다른 복장도 가죽제로 바꿔보았다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>파자마 갑옷</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>회복약</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>회복약 G</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>회복약 GG</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>회복약 GGG</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>약초를 달여서 만든 회복약. 쓰디 쓰고 쓴데 씁다. 한 마디로 매우 쓰다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>회복약에 벌꿀을 넣고 달인 약. 벌꿀을 넣었는데도 회복약 보다 더 쓰다. 분명 벌꿀 말고 다른 게 들어갔다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>회복약을 더욱 달인 약. 이번에는 대추야자를 넣었다. 제발 그만 좀 써져라.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>회복약에 쑥을 넣고 극도로 달인 약. 이젠 고약이나 다름 없다. 이젠 너무 달다. 살려줘.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>안에 인화성 액체가 들어있는 병. 왜인지는 몰라도 절대로 안깨진다. 액체는 거들 뿐이다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>화염병</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>널부러진 돌맹이와는 차원을 달리하는 레어 돌맹이. 맞으면 아프다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>짱돌</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>슬라임의 체액으로 만들어진 갑옷. 투명한 재질인데다 촉감도 요상하다 보니 보통 잠옷 위에 겹쳐입는다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>토끼 농부들이 사용하는 낫. 낮에는 밭을 매고 밤에는 수렵하는... 그들은 '노동자'다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -407,7 +491,7 @@
         <family val="2"/>
         <charset val="129"/>
       </rPr>
-      <t>토끼들이 자주 사용하는 호미. 낮에는 밭을 매고, 밤에는 수렵하는…</t>
+      <t>토끼들이 자주 사용하는 호미. 낮에는 밭을 매고 밤에는 수렵하는…</t>
     </r>
     <r>
       <rPr>
@@ -422,100 +506,83 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FF000000"/>
-        <rFont val="Arial Unicode MS"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>이런 말 안듣는 아이들…</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>초보 모험가들이 자주 입는 복장. 초록색 옷에 초록색 모자가 특징이다. 전설 같은 건 없다.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>모험가 복장</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>가격이 있어서 베테랑 모험가들이 자주 입는다. 푸른 상의가 특징이다. 자꾸 전설을 찾지 말아라.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>탐험가 복장</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>보랏빛 허리 망토가 특징인 장비. 세상을 구한 영웅의 옷을 모방했다는 전설이 있다.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>구원자 복장</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>늑대 가죽</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>늑대들의 가죽을 그대로 뒤집어 쓴 것. 느낌을 살리기 위해서 다른 복장도 가죽제로 바꿔보았다.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>파자마 갑옷</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>회복약</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>회복약 G</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>회복약 GG</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>회복약 GGG</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>약초를 달여서 만든 회복약. 쓰디 쓰고 쓴데 씁다. 한 마디로 매우 쓰다.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>회복약에 벌꿀을 넣고 달인 약. 벌꿀을 넣었는데도 회복약 보다 더 쓰다. 분명 벌꿀 말고 다른 게 들어갔다.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>회복약을 더욱 달인 약. 이번에는 대추야자를 넣었다. 제발 그만 좀 써져라.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>회복약에 쑥을 넣고 극도로 달인 약. 이젠 고약이나 다름 없다. 이젠 너무 달다. 살려줘.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>안에 인화성 액체가 들어있는 병. 왜인지는 몰라도 절대로 안깨진다. 액체는 거들 뿐이다.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>화염병</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>널부러진 돌맹이와는 차원을 달리하는 레어 돌맹이. 맞으면 아프다.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>짱돌</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>슬라임의 체액으로 만들어진 갑옷. 투명한 재질인데다 촉감도 요상하다 보니 보통 잠옷 위에 겹쳐입는다.</t>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>이런</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>말</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>안듣는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>아이들</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>…</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>커트시를 하는 듯 우아한 움직임으로 사용하는 고양이 일족의 무기.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -608,15 +675,15 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="3"/>
       <charset val="129"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="3"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
       <charset val="129"/>
     </font>
   </fonts>
@@ -669,7 +736,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -897,7 +964,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -907,7 +974,7 @@
     <col min="7" max="9" width="12.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="12.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1040,13 +1107,13 @@
         <v>1</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="G5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="I5" s="2">
         <v>0</v>
@@ -1069,13 +1136,13 @@
         <v>1</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="G6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="I6" s="2">
         <v>0</v>
@@ -1098,10 +1165,10 @@
         <v>1</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I7" s="2">
         <v>1</v>
@@ -1124,10 +1191,10 @@
         <v>1</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I8" s="2">
         <v>1</v>
@@ -1150,10 +1217,10 @@
         <v>1</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I9" s="2">
         <v>1</v>
@@ -1176,10 +1243,10 @@
         <v>1</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H10" s="2">
         <v>6000</v>
@@ -1205,10 +1272,10 @@
         <v>1</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H11" s="2">
         <v>6001</v>
@@ -1234,10 +1301,10 @@
         <v>1</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H12" s="2">
         <v>6002</v>
@@ -1263,10 +1330,10 @@
         <v>1</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H13" s="2">
         <v>6003</v>
@@ -1292,10 +1359,10 @@
         <v>1</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H14" s="2">
         <v>5001</v>
@@ -1408,13 +1475,13 @@
         <v>1</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I18" s="2">
         <v>0</v>
@@ -1437,13 +1504,13 @@
         <v>1</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I19" s="2">
         <v>0</v>
@@ -1466,10 +1533,10 @@
         <v>1</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I20" s="2">
         <v>1</v>
@@ -1492,10 +1559,10 @@
         <v>1</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I21" s="2">
         <v>1</v>
@@ -1518,10 +1585,10 @@
         <v>1</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H22" s="2">
         <v>5000</v>

</xml_diff>

<commit_message>
[Update] xlsx files & csv files
remove Consumable attack items
Change Consumable recover items' status's effect
</commit_message>
<xml_diff>
--- a/Documents/Files/Item.xlsx
+++ b/Documents/Files/Item.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sparta_Coding_Club\TeamProject\TextRPG_TeamProject2nd\TextRPG_TeamProject2nd\Documents\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0F9F7E-271E-426D-B490-740EAA818A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916B8E93-D3B7-4B2A-BA36-3625BDCDD471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28695" yWindow="16110" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -437,22 +437,6 @@
   </si>
   <si>
     <t>회복약에 쑥을 넣고 극도로 달인 약. 이젠 고약이나 다름 없다. 이젠 너무 달다. 살려줘.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>안에 인화성 액체가 들어있는 병. 왜인지는 몰라도 절대로 안깨진다. 액체는 거들 뿐이다.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>화염병</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>널부러진 돌맹이와는 차원을 달리하는 레어 돌맹이. 맞으면 아프다.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>짱돌</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -960,11 +944,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1017,7 +1001,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>9</v>
@@ -1046,7 +1030,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>13</v>
@@ -1075,7 +1059,7 @@
         <v>500</v>
       </c>
       <c r="E4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>15</v>
@@ -1104,10 +1088,10 @@
         <v>500</v>
       </c>
       <c r="E5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>25</v>
@@ -1133,10 +1117,10 @@
         <v>500</v>
       </c>
       <c r="E6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>28</v>
@@ -1162,7 +1146,7 @@
         <v>100</v>
       </c>
       <c r="E7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>33</v>
@@ -1188,7 +1172,7 @@
         <v>250</v>
       </c>
       <c r="E8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>35</v>
@@ -1214,7 +1198,7 @@
         <v>500</v>
       </c>
       <c r="E9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>37</v>
@@ -1237,19 +1221,16 @@
         <v>0</v>
       </c>
       <c r="D10" s="2">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="E10" s="2">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>46</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>42</v>
-      </c>
-      <c r="H10" s="2">
-        <v>6000</v>
       </c>
       <c r="I10" s="2">
         <v>2</v>
@@ -1266,19 +1247,16 @@
         <v>0</v>
       </c>
       <c r="D11" s="2">
-        <v>65</v>
+        <v>250</v>
       </c>
       <c r="E11" s="2">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>47</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="H11" s="2">
-        <v>6001</v>
       </c>
       <c r="I11" s="2">
         <v>2</v>
@@ -1295,19 +1273,16 @@
         <v>0</v>
       </c>
       <c r="D12" s="2">
-        <v>135</v>
+        <v>600</v>
       </c>
       <c r="E12" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>48</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="H12" s="2">
-        <v>6002</v>
       </c>
       <c r="I12" s="2">
         <v>2</v>
@@ -1324,10 +1299,10 @@
         <v>0</v>
       </c>
       <c r="D13" s="2">
-        <v>295</v>
+        <v>1500</v>
       </c>
       <c r="E13" s="2">
-        <v>1</v>
+        <v>150</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>49</v>
@@ -1335,45 +1310,42 @@
       <c r="G13" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="2">
-        <v>6003</v>
-      </c>
       <c r="I13" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1">
       <c r="A14" s="2">
-        <v>1204</v>
+        <v>2000</v>
       </c>
       <c r="B14" s="2">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C14" s="2">
         <v>0</v>
       </c>
       <c r="D14" s="2">
-        <v>80</v>
+        <v>250</v>
       </c>
       <c r="E14" s="2">
-        <v>1</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="H14" s="2">
-        <v>5001</v>
+        <v>0</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I14" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1">
       <c r="A15" s="2">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="B15" s="2">
         <v>50</v>
@@ -1385,16 +1357,16 @@
         <v>250</v>
       </c>
       <c r="E15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="I15" s="2">
         <v>0</v>
@@ -1402,28 +1374,28 @@
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1">
       <c r="A16" s="2">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="B16" s="2">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C16" s="2">
-        <v>0</v>
+        <v>-35</v>
       </c>
       <c r="D16" s="2">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="E16" s="2">
-        <v>1</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>20</v>
+        <v>0</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I16" s="2">
         <v>0</v>
@@ -1431,28 +1403,28 @@
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1">
       <c r="A17" s="2">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="B17" s="2">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="C17" s="2">
-        <v>-35</v>
+        <v>20</v>
       </c>
       <c r="D17" s="2">
         <v>500</v>
       </c>
       <c r="E17" s="2">
-        <v>1</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>22</v>
+        <v>0</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="I17" s="2">
         <v>0</v>
@@ -1460,28 +1432,28 @@
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1">
       <c r="A18" s="2">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="B18" s="2">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C18" s="2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D18" s="2">
         <v>500</v>
       </c>
       <c r="E18" s="2">
-        <v>1</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>24</v>
+        <v>0</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="I18" s="2">
         <v>0</v>
@@ -1489,112 +1461,54 @@
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1">
       <c r="A19" s="2">
-        <v>2004</v>
+        <v>2100</v>
       </c>
       <c r="B19" s="2">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="C19" s="2">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="D19" s="2">
         <v>500</v>
       </c>
       <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" s="2">
         <v>1</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I19" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1">
       <c r="A20" s="2">
-        <v>2100</v>
+        <v>2101</v>
       </c>
       <c r="B20" s="2">
-        <v>15</v>
+        <v>-35</v>
       </c>
       <c r="C20" s="2">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="D20" s="2">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="E20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I20" s="2">
         <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A21" s="2">
-        <v>2101</v>
-      </c>
-      <c r="B21" s="2">
-        <v>-35</v>
-      </c>
-      <c r="C21" s="2">
-        <v>100</v>
-      </c>
-      <c r="D21" s="2">
-        <v>1000</v>
-      </c>
-      <c r="E21" s="2">
-        <v>1</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="I21" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A22" s="2">
-        <v>2200</v>
-      </c>
-      <c r="B22" s="2">
-        <v>0</v>
-      </c>
-      <c r="C22" s="2">
-        <v>0</v>
-      </c>
-      <c r="D22" s="2">
-        <v>45</v>
-      </c>
-      <c r="E22" s="2">
-        <v>1</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H22" s="2">
-        <v>5000</v>
-      </c>
-      <c r="I22" s="2">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>